<commit_message>
Updating paper backup for the first draft. Closes xwsxethan/MusicScoring#93
</commit_message>
<xml_diff>
--- a/Documents/Data/Graded Pieces and Complexity Scores.xlsx
+++ b/Documents/Data/Graded Pieces and Complexity Scores.xlsx
@@ -4,10 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="23560" windowHeight="16900" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GradeComplexity" sheetId="3" r:id="rId1"/>
+    <sheet name="AveGradeComplexity" sheetId="4" r:id="rId2"/>
+    <sheet name="AveGradeComplexityScaled" sheetId="5" r:id="rId3"/>
+    <sheet name="Datasheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
   <si>
     <t>Grade</t>
   </si>
@@ -153,9 +157,6 @@
     <t>Sonata 1st Movement</t>
   </si>
   <si>
-    <t>Saint Saens</t>
-  </si>
-  <si>
     <t>Sonata 3rd and 4th Movements</t>
   </si>
   <si>
@@ -177,32 +178,146 @@
     <t>Messager</t>
   </si>
   <si>
-    <t>Stanford Sonata no. 2 1st Movement</t>
-  </si>
-  <si>
-    <t>Charles Villiers</t>
-  </si>
-  <si>
     <t>Eerie Canal Capers</t>
+  </si>
+  <si>
+    <t>Sonata no. 2 1st Movement</t>
+  </si>
+  <si>
+    <t>Ready?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Alouette.xml</t>
+  </si>
+  <si>
+    <t>Bingo.xml</t>
+  </si>
+  <si>
+    <t>Charles Villiers Stanford Sonata op 129 1st Movement.xml</t>
+  </si>
+  <si>
+    <t>Crussell Concerto no 3 1st and 2nd Movements.xml</t>
+  </si>
+  <si>
+    <t>Crussell Concerto no 3 2nd and 3rd Movements.xml</t>
+  </si>
+  <si>
+    <t>ErieCanalCapers.xml</t>
+  </si>
+  <si>
+    <t>Gavotte.xml</t>
+  </si>
+  <si>
+    <t>Go for Excellence no. 61.xml</t>
+  </si>
+  <si>
+    <t>Grandfathers Whiskers.xml</t>
+  </si>
+  <si>
+    <t>Hindemith Clarinet Sonata 2nd Movement.xml</t>
+  </si>
+  <si>
+    <t>Hindemith Clarinet Sonata 3rd and 4th Movement.xml</t>
+  </si>
+  <si>
+    <t>Hymn to the Sun.xml</t>
+  </si>
+  <si>
+    <t>Just Fine.xml</t>
+  </si>
+  <si>
+    <t>Krommer concerto op 36 1st Movement.xml</t>
+  </si>
+  <si>
+    <t>Loch Lomond.xml</t>
+  </si>
+  <si>
+    <t>Messager Solo de Concours.xml</t>
+  </si>
+  <si>
+    <t>Ming Court.xml</t>
+  </si>
+  <si>
+    <t>Minuet in G.xml</t>
+  </si>
+  <si>
+    <t>Nocturne.xml</t>
+  </si>
+  <si>
+    <t>pierne canzonetta.xml</t>
+  </si>
+  <si>
+    <t>Promenade.xml</t>
+  </si>
+  <si>
+    <t>Rabaud Solo de Concors.xml</t>
+  </si>
+  <si>
+    <t>Saint Saens Clarinet Sonata 1st Movement.xml</t>
+  </si>
+  <si>
+    <t>Saint Saens Clarinet Sonata 2nd 3rd and 4th Movements.xml</t>
+  </si>
+  <si>
+    <t>Scene and Air.xml</t>
+  </si>
+  <si>
+    <t>Scherzo.xml</t>
+  </si>
+  <si>
+    <t>Serenade.xml</t>
+  </si>
+  <si>
+    <t>Song without Words.xml</t>
+  </si>
+  <si>
+    <t>Theme from Symphony 9 by Beethoven.xml</t>
+  </si>
+  <si>
+    <t>Variations on a Theme by Mozart.xml</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Korsakoff</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>Saint-Saens</t>
+  </si>
+  <si>
+    <t>Poldini</t>
+  </si>
+  <si>
+    <t>Dvorak</t>
+  </si>
+  <si>
+    <t>Tschaikowsky</t>
+  </si>
+  <si>
+    <t>Better Names</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -238,36 +353,125 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -279,6 +483,49 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -290,11 +537,673 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="116"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="16"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Datasheet!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Datasheet!$C$2:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>535.216216216216</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>646.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>551.303571428571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1019.97573333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1546.47428571428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>639.256129032259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>887.843478260868</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>514.191780821917</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1020.793125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2326.87441860465</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9464.1992307692</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16344.7199817351</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15339.2669023255</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35333.655653513</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5688.39402409639</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11433.8131455399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8176.83285411871</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4878.22716777407</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26753.3227707808</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10053.2100365408</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15123.1998654797</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41135.230425815</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14072.6896603382</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>109410.145033738</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11040.1588744542</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14250.7323706896</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>51606.374351382</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46079.2507024443</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59215.2618293637</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>202214.848193578</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36076.391025145</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37601.3884283725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2118856520"/>
+        <c:axId val="2118859560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2118856520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2118859560"/>
+        <c:crossesAt val="0.0"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118859560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2118856520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="116"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="16"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Datasheet!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>577.7732625482623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1068.568716026623</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1187.425700671859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13716.0620382766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17485.28760771643</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12465.39820730359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28129.21514564735</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44840.9978561768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37312.1191415053</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83776.9723691148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2118927896"/>
+        <c:axId val="2118930696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2118927896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2118930696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118930696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2118927896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="116"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="16"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Datasheet!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>577.7732625482623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1068.568716026623</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1187.425700671859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13716.0620382766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17485.28760771643</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12465.39820730359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28129.21514564735</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44840.9978561768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37312.1191415053</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83776.9723691148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2118962520"/>
+        <c:axId val="2118965320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2118962520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118965320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118965320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="250000.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2118962520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8584088" cy="5840146"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8584088" cy="5840146"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8584088" cy="5840146"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,540 +1528,952 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:9">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" ht="16">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1">
+        <v>535.21621621621603</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" ht="16">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="str">
+        <f>D2 &amp; " by " &amp; E2</f>
+        <v>Bingo by Standard of Excellence</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(B$2:B$33,J2,C$2:C$33)/COUNTIF(B$2:B$33,J2)</f>
+        <v>577.77326254826232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="2"/>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>54</v>
+      <c r="C3" s="1">
+        <v>646.79999999999995</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" ht="16">
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H33" si="0">D3 &amp; " by " &amp; E3</f>
+        <v>Eerie Canal Capers by Standard of Excellence</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K11" si="1">SUMIF(B$2:B$33,J3,C$2:C$33)/COUNTIF(B$2:B$33,J3)</f>
+        <v>1068.5687160266232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="2"/>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1">
+        <v>551.30357142857099</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="2:9" ht="16">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>Go for Excellence no. 61 by Standard of Excellence</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>1187.4257006718587</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1">
+        <v>1019.97573333333</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="2:9" ht="16">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>Alouette by Standard of Excellence</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>13716.062038276599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="2"/>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1">
+        <v>1546.4742857142801</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="2:9" ht="16">
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>Grandfather's Whiskers by Standard of Excellence</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>17485.287607716429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="2"/>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1">
+        <v>639.25612903225897</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="2:9" ht="16">
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>Ming Court by Standard of Excellence</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>12465.398207303595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1">
+        <v>887.84347826086798</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="2:9" ht="16">
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>Just Fine by Standard of Excellence</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>28129.215145647351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="2"/>
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1">
+        <v>514.19178082191695</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="2:9" ht="16">
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>Variations on a Theme by Mozart</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>44840.9978561768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="2"/>
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1">
+        <v>1020.793125</v>
+      </c>
+      <c r="D10" t="s">
         <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="2:9">
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>Loch Lomond by Standard of Excellence</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>37312.119141505304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="2"/>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1">
+        <v>2326.8744186046501</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>Theme from Symphony 9 by Beethoven</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>83776.972369114796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1">
+        <v>9464.1992307691999</v>
+      </c>
+      <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>Minuet in G by Beethoven</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2"/>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1">
+        <v>16344.719981735099</v>
+      </c>
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>7</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>Gavotte by Gossec</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="2"/>
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1">
+        <v>15339.2669023255</v>
+      </c>
+      <c r="D14" t="s">
         <v>23</v>
       </c>
       <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
         <v>7</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>Song without Words by Tschaikowsky</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1">
+        <v>35333.655653513</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9">
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>Humoresque by Dvorak</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2"/>
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1">
+        <v>5688.3940240963902</v>
+      </c>
+      <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>The Dancing Doll by Poldini</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2"/>
       <c r="B17">
         <v>5</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1">
+        <v>11433.8131455399</v>
+      </c>
+      <c r="D17" t="s">
         <v>26</v>
       </c>
       <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
         <v>7</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>Hymn to the Sun by Korsakoff</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>6</v>
+      </c>
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1">
+        <v>8176.8328541187102</v>
+      </c>
+      <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>28</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>7</v>
       </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>Serenade by Drdla</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2"/>
       <c r="B19">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1">
+        <v>4878.22716777407</v>
+      </c>
+      <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>30</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>8</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>Promenade by Delmas</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2"/>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1">
+        <v>26753.3227707808</v>
+      </c>
+      <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="G20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>Scherzo by Koepke</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2"/>
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1">
+        <v>10053.210036540801</v>
+      </c>
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>34</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>8</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>Nocturne by Bassi</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="2">
+        <v>7</v>
+      </c>
       <c r="B22">
         <v>7</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1">
+        <v>15123.199865479701</v>
+      </c>
+      <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>36</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>9</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
+      <c r="G22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonata 2nd Movement by Hindemith</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2"/>
       <c r="B23">
         <v>7</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1">
+        <v>41135.230425815003</v>
+      </c>
+      <c r="D23" t="s">
         <v>37</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>38</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>8</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>Scene and Air by Bergsen</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2">
+        <v>8</v>
+      </c>
       <c r="B24">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1">
+        <v>14072.689660338199</v>
+      </c>
+      <c r="D24" t="s">
         <v>39</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>40</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>9</v>
       </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>Canzonetta by Pierné</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2"/>
       <c r="B25">
         <v>8</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1">
+        <v>109410.14503373799</v>
+      </c>
+      <c r="D25" t="s">
         <v>41</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>9</v>
       </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>Concerto Opus 36 1st Movement by Krommer</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2"/>
       <c r="B26">
         <v>8</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1">
+        <v>11040.1588744542</v>
+      </c>
+      <c r="D26" t="s">
         <v>43</v>
       </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
       <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
         <v>9</v>
       </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonata 1st Movement by Saint-Saens</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="2">
+        <v>9</v>
+      </c>
       <c r="B27">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
-        <v>45</v>
+      <c r="C27" s="1">
+        <v>14250.7323706896</v>
       </c>
       <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
         <v>36</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>9</v>
       </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonata 3rd and 4th Movements by Hindemith</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="2"/>
       <c r="B28">
         <v>9</v>
       </c>
-      <c r="C28" t="s">
-        <v>46</v>
+      <c r="C28" s="1">
+        <v>51606.374351382001</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
         <v>9</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonata Movements 2, 3, and 4 by Saint-Saens</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2"/>
       <c r="B29">
         <v>9</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1">
+        <v>46079.250702444297</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
         <v>47</v>
       </c>
-      <c r="D29" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>9</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>Solo de Concours by Rabaud</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="2">
+        <v>10</v>
+      </c>
       <c r="B30">
         <v>10</v>
       </c>
-      <c r="C30" t="s">
-        <v>49</v>
+      <c r="C30" s="1">
+        <v>59215.261829363699</v>
       </c>
       <c r="D30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
         <v>36</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>9</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
+      <c r="G30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>Concerto no. 3 1st and 2nd Movements by Hindemith</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2"/>
       <c r="B31">
         <v>10</v>
       </c>
-      <c r="C31" t="s">
-        <v>50</v>
+      <c r="C31" s="1">
+        <v>202214.84819357799</v>
       </c>
       <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
         <v>36</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>9</v>
       </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>Concerto no. 3 2nd and 3rd Movements by Hindemith</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="2"/>
       <c r="B32">
         <v>10</v>
       </c>
-      <c r="C32" t="s">
-        <v>47</v>
+      <c r="C32" s="1">
+        <v>36076.391025145</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
         <v>9</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>Solo de Concours by Messager</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="2"/>
       <c r="B33">
         <v>10</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1">
+        <v>37601.388428372498</v>
+      </c>
+      <c r="D33" t="s">
         <v>52</v>
       </c>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
       <c r="E33" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" t="s">
         <v>9</v>
       </c>
-      <c r="F33">
-        <v>0</v>
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>Sonata no. 2 1st Movement by Stanford</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A21"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1161,4 +2482,264 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2">
+        <v>1019.97573333333</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>535.21621621621603</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <v>37601.388428372498</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>59215.261829363699</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6">
+        <v>202214.84819357799</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>646.79999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8">
+        <v>16344.719981735099</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9">
+        <v>551.30357142857099</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10">
+        <v>1546.4742857142801</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>15123.199865479701</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12">
+        <v>14250.7323706896</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>11433.8131455399</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>887.84347826086798</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15">
+        <v>109410.14503373799</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>1020.793125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17">
+        <v>36076.391025145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18">
+        <v>639.25612903225897</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19">
+        <v>9464.1992307691999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20">
+        <v>10053.210036540801</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21">
+        <v>14072.689660338199</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22">
+        <v>4878.22716777407</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23">
+        <v>46079.250702444297</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24">
+        <v>11040.1588744542</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25">
+        <v>51606.374351382001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>41135.230425815003</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27">
+        <v>26753.3227707808</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28">
+        <v>8176.8328541187102</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29">
+        <v>15339.2669023255</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30">
+        <v>2326.8744186046501</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31">
+        <v>514.19178082191695</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Crussell's name being reported as Hindemith and updated the paper backup since Chrome is lagging out.
</commit_message>
<xml_diff>
--- a/Documents/Data/Graded Pieces and Complexity Scores.xlsx
+++ b/Documents/Data/Graded Pieces and Complexity Scores.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="99">
   <si>
     <t>Grade</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>2nd Max</t>
+  </si>
+  <si>
+    <t>Crussell</t>
   </si>
 </sst>
 </file>
@@ -369,8 +372,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -503,7 +508,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -566,6 +571,7 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -628,6 +634,7 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1817,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2788,7 +2795,7 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
@@ -2798,7 +2805,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>Concerto no. 3 1st and 2nd Movements by Hindemith</v>
+        <v>Concerto no. 3 1st and 2nd Movements by Crussell</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2813,7 +2820,7 @@
         <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
@@ -2823,7 +2830,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>Concerto no. 3 2nd and 3rd Movements by Hindemith</v>
+        <v>Concerto no. 3 2nd and 3rd Movements by Crussell</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2913,6 +2920,15 @@
       <c r="D37" t="str">
         <f>INDEX(D$2:D$33,MATCH(C37,C$2:C$33))</f>
         <v>Concerto Opus 36 1st Movement</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="C38" s="1">
+        <f>SMALL(C2:C33,2)</f>
+        <v>535.21621621621603</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding in some changes as per the recommendations of the ONWARD! reviewers. Preparing for resubmission.
</commit_message>
<xml_diff>
--- a/Documents/Data/Graded Pieces and Complexity Scores.xlsx
+++ b/Documents/Data/Graded Pieces and Complexity Scores.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="480" windowWidth="23560" windowHeight="16900" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="840" yWindow="480" windowWidth="26920" windowHeight="16900" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GradeComplexity" sheetId="3" r:id="rId1"/>
     <sheet name="AveGradeComplexityScaled" sheetId="5" r:id="rId2"/>
     <sheet name="AveGradeComplexity" sheetId="4" r:id="rId3"/>
-    <sheet name="AveComplexityOverGrade" sheetId="6" r:id="rId4"/>
-    <sheet name="Datasheet" sheetId="1" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
+    <sheet name="AveGradeComplexityTrendline" sheetId="9" r:id="rId4"/>
+    <sheet name="AveComplexityOverGrade" sheetId="6" r:id="rId5"/>
+    <sheet name="AllPiecesLinearRegression" sheetId="7" r:id="rId6"/>
+    <sheet name="AverageLinearRegression" sheetId="8" r:id="rId7"/>
+    <sheet name="Datasheet" sheetId="1" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="108">
   <si>
     <t>Grade</t>
   </si>
@@ -321,14 +324,42 @@
   </si>
   <si>
     <t>Crussell</t>
+  </si>
+  <si>
+    <t>All Pieces</t>
+  </si>
+  <si>
+    <t>Averages</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>e^2</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>y-intercept</t>
+  </si>
+  <si>
+    <t>R-squared</t>
+  </si>
+  <si>
+    <t>MSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -363,7 +394,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -371,8 +402,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -500,15 +611,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -572,6 +705,12 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -635,6 +774,12 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,7 +817,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Datasheet!$A$2:$A$33</c:f>
+              <c:f>Datasheet!$D$2:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -711,7 +856,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Datasheet!$C$2:$C$33</c:f>
+              <c:f>Datasheet!$F$2:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="32"/>
@@ -825,11 +970,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118856520"/>
-        <c:axId val="2118859560"/>
+        <c:axId val="2111778584"/>
+        <c:axId val="2097216008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118856520"/>
+        <c:axId val="2111778584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +994,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118859560"/>
+        <c:crossAx val="2097216008"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -857,7 +1002,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118859560"/>
+        <c:axId val="2097216008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,7 +1023,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118856520"/>
+        <c:crossAx val="2111778584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -917,7 +1062,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Datasheet!$K$2:$K$11</c:f>
+              <c:f>Datasheet!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -964,11 +1109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118962520"/>
-        <c:axId val="2118965320"/>
+        <c:axId val="2086794744"/>
+        <c:axId val="2086797688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118962520"/>
+        <c:axId val="2086794744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +1122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118965320"/>
+        <c:crossAx val="2086797688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -985,7 +1130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118965320"/>
+        <c:axId val="2086797688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250000.0"/>
@@ -997,7 +1142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118962520"/>
+        <c:crossAx val="2086794744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1040,7 +1185,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Datasheet!$L$2:$L$11</c:f>
+                <c:f>Datasheet!$P$2:$P$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -1079,7 +1224,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Datasheet!$L$2:$L$11</c:f>
+                <c:f>Datasheet!$P$2:$P$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -1119,7 +1264,7 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Datasheet!$K$2:$K$11</c:f>
+              <c:f>Datasheet!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1166,11 +1311,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118927896"/>
-        <c:axId val="2118930696"/>
+        <c:axId val="2097398440"/>
+        <c:axId val="2097401448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118927896"/>
+        <c:axId val="2097398440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,7 +1336,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118930696"/>
+        <c:crossAx val="2097401448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1199,7 +1344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118930696"/>
+        <c:axId val="2097401448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,7 +1365,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118927896"/>
+        <c:crossAx val="2097398440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1257,9 +1402,97 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Datasheet!$P$2:$P$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>49.24915303404015</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>371.9607097787382</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>683.5757483437636</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3034.412296104154</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>12836.81273120191</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8454.590428790688</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>13006.01528016765</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>45674.0636552081</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16462.23848291448</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>9197.62164532783</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Datasheet!$P$2:$P$11</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>49.24915303404015</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>371.9607097787382</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>683.5757483437636</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3034.412296104154</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>12836.81273120191</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8454.590428790688</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>13006.01528016765</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>45674.0636552081</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>16462.23848291448</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>9197.62164532783</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Datasheet!$M$2:$M$11</c:f>
+              <c:f>Datasheet!$O$2:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1267,31 +1500,31 @@
                   <c:v>577.7732625482623</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>534.2843580133115</c:v>
+                  <c:v>1068.568716026623</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>395.8085668906196</c:v>
+                  <c:v>1187.425700671859</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3429.01550956915</c:v>
+                  <c:v>13716.0620382766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3497.057521543286</c:v>
+                  <c:v>17485.28760771643</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2077.566367883932</c:v>
+                  <c:v>12465.39820730359</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4018.45930652105</c:v>
+                  <c:v>28129.21514564735</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5605.1247320221</c:v>
+                  <c:v>44840.9978561768</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4145.791015722812</c:v>
+                  <c:v>37312.1191415053</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8377.69723691148</c:v>
+                  <c:v>83776.9723691148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,11 +1539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2137347672"/>
-        <c:axId val="2137349080"/>
+        <c:axId val="2109554104"/>
+        <c:axId val="2109557912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2137347672"/>
+        <c:axId val="2109554104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1318,8 +1551,20 @@
         <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137349080"/>
+        <c:tickLblPos val="low"/>
+        <c:txPr>
+          <a:bodyPr lIns="0" anchor="t" anchorCtr="1">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2109557912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1572,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137349080"/>
+        <c:axId val="2109557912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,11 +1583,655 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2137347672"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2109554104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="116"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="16"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Datasheet!$Q$2:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>577.7732625482623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>534.2843580133115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>395.8085668906196</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3429.01550956915</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3497.057521543286</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2077.566367883932</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4018.45930652105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5605.1247320221</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4145.791015722812</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8377.69723691148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2097328152"/>
+        <c:axId val="2097331096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2097328152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2097331096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2097331096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2097328152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Datasheet!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Complexity Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.278009382010063"/>
+                  <c:y val="-0.289283863793816"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Datasheet!$E$2:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Datasheet!$F$2:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>535.216216216216</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>646.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>551.303571428571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1019.97573333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1546.47428571428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>639.256129032259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>887.843478260868</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>514.191780821917</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1020.793125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2326.87441860465</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9464.1992307692</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16344.7199817351</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15339.2669023255</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35333.655653513</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5688.39402409639</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11433.8131455399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8176.83285411871</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4878.22716777407</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>26753.3227707808</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10053.2100365408</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15123.1998654797</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41135.230425815</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14072.6896603382</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>109410.145033738</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11040.1588744542</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14250.7323706896</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>51606.374351382</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>46079.2507024443</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>59215.2618293637</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>202214.848193578</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36076.391025145</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37601.3884283725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2084155080"/>
+        <c:axId val="2106506072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2084155080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2106506072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2106506072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2084155080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Datasheet!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.291025557985892"/>
+                  <c:y val="-0.00702037243589458"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Datasheet!$N$2:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Datasheet!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>577.7732625482623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1068.568716026623</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1187.425700671859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13716.0620382766</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17485.28760771643</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12465.39820730359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28129.21514564735</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44840.9978561768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37312.1191415053</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83776.9723691148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2108911864"/>
+        <c:axId val="2108940872"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2108911864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2108940872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2108940872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2108911864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1387,7 +2276,40 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="153" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1476,6 +2398,87 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8584088" cy="5840146"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8584088" cy="5840146"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8584088" cy="5840146"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -1824,1125 +2827,1702 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>92</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="2">
+      <c r="S1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" t="s">
+        <v>101</v>
+      </c>
+      <c r="U1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <f>E2*$Q$19+$Q$20</f>
+        <v>-11966.326815008662</v>
+      </c>
+      <c r="B2" s="1">
+        <f>F2-A2</f>
+        <v>12501.543031224879</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2^2</f>
+        <v>156288578.16156733</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="F2" s="1">
         <v>535.21621621621603</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" t="str">
-        <f>D2 &amp; " by " &amp; E2</f>
+      <c r="K2" t="str">
+        <f>G2 &amp; " by " &amp; H2</f>
         <v>Bingo by Standard of Excellence</v>
       </c>
-      <c r="J2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="K2">
-        <f>SUMIF(B$2:B$33,J2,C$2:C$33)/COUNTIF(B$2:B$33,J2)</f>
+      <c r="O2">
+        <f>SUMIF(E$2:E$33,N2,F$2:F$33)/COUNTIF(E$2:E$33,N2)</f>
         <v>577.77326254826232</v>
       </c>
-      <c r="L2">
-        <f>_xlfn.STDEV.P(C2:C4)</f>
+      <c r="P2">
+        <f>_xlfn.STDEV.P(F2:F4)</f>
         <v>49.249153034040155</v>
       </c>
-      <c r="M2">
-        <f>K2/J2</f>
+      <c r="Q2">
+        <f>O2/N2</f>
         <v>577.77326254826232</v>
       </c>
-      <c r="N2">
-        <f>(K3-K2)/K2</f>
+      <c r="R2">
+        <f t="shared" ref="R2:R11" si="0">(O3-O2)/O2</f>
         <v>0.84946030786144922</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="2"/>
-      <c r="B3">
+      <c r="S2">
+        <f>N2*$R$19+$R$20</f>
+        <v>-10279.974603774157</v>
+      </c>
+      <c r="T2">
+        <f>O2-S2</f>
+        <v>10857.747866322419</v>
+      </c>
+      <c r="U2">
+        <f>T2^2</f>
+        <v>117890688.72862905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <f>E3*$Q$19+$Q$20</f>
+        <v>-11966.326815008662</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B33" si="1">F3-A3</f>
+        <v>12613.126815008662</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C33" si="2">B3^2</f>
+        <v>159090968.05149055</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="F3" s="1">
         <v>646.79999999999995</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>54</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H33" si="0">D3 &amp; " by " &amp; E3</f>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K33" si="3">G3 &amp; " by " &amp; H3</f>
         <v>Eerie Canal Capers by Standard of Excellence</v>
       </c>
-      <c r="J3">
+      <c r="N3">
         <v>2</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K11" si="1">SUMIF(B$2:B$33,J3,C$2:C$33)/COUNTIF(B$2:B$33,J3)</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="4">SUMIF(E$2:E$33,N3,F$2:F$33)/COUNTIF(E$2:E$33,N3)</f>
         <v>1068.5687160266232</v>
       </c>
-      <c r="L3">
-        <f>_xlfn.STDEV.P(C5:C7)</f>
+      <c r="P3">
+        <f>_xlfn.STDEV.P(F5:F7)</f>
         <v>371.96070977873819</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M11" si="2">K3/J3</f>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q11" si="5">O3/N3</f>
         <v>534.28435801331159</v>
       </c>
-      <c r="N3">
-        <f>(K4-K3)/K3</f>
+      <c r="R3">
+        <f t="shared" si="0"/>
         <v>0.11123008081987895</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="2"/>
-      <c r="B4">
+      <c r="S3">
+        <f>N3*$R$19+$R$20</f>
+        <v>-2649.7620241579516</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T11" si="6">O3-S3</f>
+        <v>3718.330740184575</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U11" si="7">T3^2</f>
+        <v>13825983.49340157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <f>E4*$Q$19+$Q$20</f>
+        <v>-11966.326815008662</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="1"/>
+        <v>12517.630386437233</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="2"/>
+        <v>156691070.49145675</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="F4" s="1">
         <v>551.30357142857099</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>54</v>
       </c>
-      <c r="H4" t="str">
+      <c r="K4" t="str">
+        <f t="shared" si="3"/>
+        <v>Go for Excellence no. 61 by Standard of Excellence</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="4"/>
+        <v>1187.4257006718587</v>
+      </c>
+      <c r="P4">
+        <f>_xlfn.STDEV.P(F8:F11)</f>
+        <v>683.57574834376362</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="5"/>
+        <v>395.8085668906196</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="0"/>
-        <v>Go for Excellence no. 61 by Standard of Excellence</v>
-      </c>
-      <c r="J4">
+        <v>10.551090759207838</v>
+      </c>
+      <c r="S4">
+        <f>N4*$R$19+$R$20</f>
+        <v>4980.4505554582538</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="6"/>
+        <v>-3793.0248547863948</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="7"/>
+        <v>14387037.549027352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <f>E5*$Q$19+$Q$20</f>
+        <v>-3870.4475091694694</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="1"/>
+        <v>4890.4232425027994</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="2"/>
+        <v>23916239.490811594</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1019.97573333333</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v>Alouette by Standard of Excellence</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>13716.062038276599</v>
+      </c>
+      <c r="P5">
+        <f>_xlfn.STDEV.P(F12:F14)</f>
+        <v>3034.4122961041539</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="5"/>
+        <v>3429.0155095691498</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>0.27480377085793839</v>
+      </c>
+      <c r="S5">
+        <f>N5*$R$19+$R$20</f>
+        <v>12610.663135074457</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="6"/>
+        <v>1105.3989032021418</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="7"/>
+        <v>1221906.735200498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <f>E6*$Q$19+$Q$20</f>
+        <v>-3870.4475091694694</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>5416.9217948837495</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="2"/>
+        <v>29343041.731886581</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1546.4742857142801</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v>Grandfather's Whiskers by Standard of Excellence</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>17485.287607716429</v>
+      </c>
+      <c r="P6">
+        <f>_xlfn.STDEV.P(F15:F17)</f>
+        <v>12836.812731201913</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="5"/>
+        <v>3497.0575215432859</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>-0.28709218361369748</v>
+      </c>
+      <c r="S6">
+        <f>N6*$R$19+$R$20</f>
+        <v>20240.875714690661</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="6"/>
+        <v>-2755.5881069742318</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="7"/>
+        <v>7593265.8152978299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <f>E7*$Q$19+$Q$20</f>
+        <v>-3870.4475091694694</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="1"/>
+        <v>4509.7036382017286</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="2"/>
+        <v>20337426.904409908</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>639.25612903225897</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>Ming Court by Standard of Excellence</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>12465.398207303595</v>
+      </c>
+      <c r="P7">
+        <f>_xlfn.STDEV.P(F18:F21)</f>
+        <v>8454.5904287906887</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="5"/>
+        <v>2077.5663678839323</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>1.256583759126618</v>
+      </c>
+      <c r="S7">
+        <f>N7*$R$19+$R$20</f>
+        <v>27871.088294306868</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="6"/>
+        <v>-15405.690087003273</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="7"/>
+        <v>237335287.05679092</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <f>E8*$Q$19+$Q$20</f>
+        <v>4225.4317966697236</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="1"/>
+        <v>-3337.5883184088557</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="2"/>
+        <v>11139495.783179253</v>
+      </c>
+      <c r="D8" s="2">
         <v>3</v>
       </c>
-      <c r="K4">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>887.84347826086798</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>Just Fine by Standard of Excellence</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>28129.215145647351</v>
+      </c>
+      <c r="P8">
+        <f>_xlfn.STDEV.P(F22:F23)</f>
+        <v>13006.015280167654</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="5"/>
+        <v>4018.4593065210502</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>0.59410767858254276</v>
+      </c>
+      <c r="S8">
+        <f>N8*$R$19+$R$20</f>
+        <v>35501.300873923072</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="6"/>
+        <v>-7372.0857282757206</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="7"/>
+        <v>54347647.985046566</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9">
+        <f>E9*$Q$19+$Q$20</f>
+        <v>4225.4317966697236</v>
+      </c>
+      <c r="B9" s="1">
         <f t="shared" si="1"/>
-        <v>1187.4257006718587</v>
-      </c>
-      <c r="L4">
-        <f>_xlfn.STDEV.P(C8:C11)</f>
-        <v>683.57574834376362</v>
-      </c>
-      <c r="M4">
+        <v>-3711.2400158478067</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="2"/>
-        <v>395.8085668906196</v>
-      </c>
-      <c r="N4">
-        <f>(K5-K4)/K4</f>
-        <v>10.551090759207838</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="2">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1019.97573333333</v>
-      </c>
-      <c r="D5" t="s">
+        <v>13773302.455230029</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>514.19178082191695</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v>Variations on a Theme by Mozart</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>44840.9978561768</v>
+      </c>
+      <c r="P9">
+        <f>_xlfn.STDEV.P(F24:F26)</f>
+        <v>45674.063655208105</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>5605.1247320221</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>-0.16790167647070775</v>
+      </c>
+      <c r="S9">
+        <f>N9*$R$19+$R$20</f>
+        <v>43131.513453539272</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="6"/>
+        <v>1709.4844026375285</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="7"/>
+        <v>2922336.922860988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10">
+        <f>E10*$Q$19+$Q$20</f>
+        <v>4225.4317966697236</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>-3204.6386716697234</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="2"/>
+        <v>10269709.01596109</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1020.793125</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="3"/>
+        <v>Loch Lomond by Standard of Excellence</v>
+      </c>
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>37312.119141505304</v>
+      </c>
+      <c r="P10">
+        <f>_xlfn.STDEV.P(F27:F29)</f>
+        <v>16462.238482914483</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="5"/>
+        <v>4145.7910157228116</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>1.245301909853811</v>
+      </c>
+      <c r="S10">
+        <f>N10*$R$19+$R$20</f>
+        <v>50761.726033155486</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="6"/>
+        <v>-13449.606891650183</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="7"/>
+        <v>180891925.53992409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11">
+        <f>E11*$Q$19+$Q$20</f>
+        <v>4225.4317966697236</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>-1898.5573780650734</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="2"/>
+        <v>3604520.1178053259</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2326.8744186046501</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="3"/>
+        <v>Theme from Symphony 9 by Beethoven</v>
+      </c>
+      <c r="N11">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>83776.972369114796</v>
+      </c>
+      <c r="P11">
+        <f>_xlfn.STDEV.P(F13:F15)</f>
+        <v>9197.6216453278303</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="5"/>
+        <v>8377.6972369114792</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="S11">
+        <f>N11*$R$19+$R$20</f>
+        <v>58391.938612771686</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>25385.033756343109</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="7"/>
+        <v>644399938.8106792</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12">
+        <f>E12*$Q$19+$Q$20</f>
+        <v>12321.311102508917</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>-2857.1118717397167</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="2"/>
+        <v>8163088.2476360267</v>
+      </c>
+      <c r="D12" s="2">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E12">
         <v>4</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F12" s="1">
+        <v>9464.1992307691999</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
         <v>54</v>
       </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>Alouette by Standard of Excellence</v>
-      </c>
-      <c r="J5">
+      <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v>Minuet in G by Beethoven</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13">
+        <f>E13*$Q$19+$Q$20</f>
+        <v>12321.311102508917</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>4023.4088792261828</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="2"/>
+        <v>16187819.009436088</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13">
         <v>4</v>
       </c>
-      <c r="K5">
+      <c r="F13" s="1">
+        <v>16344.719981735099</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v>Gavotte by Gossec</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14">
+        <f>E14*$Q$19+$Q$20</f>
+        <v>12321.311102508917</v>
+      </c>
+      <c r="B14" s="1">
         <f t="shared" si="1"/>
-        <v>13716.062038276599</v>
-      </c>
-      <c r="L5">
-        <f>_xlfn.STDEV.P(C12:C14)</f>
-        <v>3034.4122961041539</v>
-      </c>
-      <c r="M5">
+        <v>3017.9557998165837</v>
+      </c>
+      <c r="C14" s="3">
         <f t="shared" si="2"/>
-        <v>3429.0155095691498</v>
-      </c>
-      <c r="N5">
-        <f>(K6-K5)/K5</f>
-        <v>0.27480377085793839</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="2"/>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1546.4742857142801</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
+        <v>9108057.2096465565</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F14" s="1">
+        <v>15339.2669023255</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
         <v>54</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>Grandfather's Whiskers by Standard of Excellence</v>
-      </c>
-      <c r="J6">
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v>Song without Words by Tschaikowsky</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15">
+        <f>E15*$Q$19+$Q$20</f>
+        <v>20417.190408348106</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>14916.465245164894</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="2"/>
+        <v>222500935.41021219</v>
+      </c>
+      <c r="D15" s="2">
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1">
+        <v>35333.655653513</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v>Humoresque by Dvorak</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16">
+        <f>E16*$Q$19+$Q$20</f>
+        <v>20417.190408348106</v>
+      </c>
+      <c r="B16" s="1">
         <f t="shared" si="1"/>
-        <v>17485.287607716429</v>
-      </c>
-      <c r="L6">
-        <f>_xlfn.STDEV.P(C15:C17)</f>
-        <v>12836.812731201913</v>
-      </c>
-      <c r="M6">
+        <v>-14728.796384251717</v>
+      </c>
+      <c r="C16" s="3">
         <f t="shared" si="2"/>
-        <v>3497.0575215432859</v>
-      </c>
-      <c r="N6">
-        <f>(K7-K6)/K6</f>
-        <v>-0.28709218361369748</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="2"/>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>639.25612903225897</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
+        <v>216937442.92874643</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5688.3940240963902</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" t="s">
         <v>54</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>Ming Court by Standard of Excellence</v>
-      </c>
-      <c r="J7">
+      <c r="K16" t="str">
+        <f t="shared" si="3"/>
+        <v>The Dancing Doll by Poldini</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17">
+        <f>E17*$Q$19+$Q$20</f>
+        <v>20417.190408348106</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="1"/>
+        <v>-8983.3772628082061</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="2"/>
+        <v>80701067.04593946</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>11433.8131455399</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="3"/>
+        <v>Hymn to the Sun by Korsakoff</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18">
+        <f>E18*$Q$19+$Q$20</f>
+        <v>28513.069714187302</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="1"/>
+        <v>-20336.236860068591</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="2"/>
+        <v>413562529.62881243</v>
+      </c>
+      <c r="D18" s="2">
         <v>6</v>
       </c>
-      <c r="K7">
+      <c r="E18">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1">
+        <v>8176.8328541187102</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="3"/>
+        <v>Serenade by Drdla</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19">
+        <f>E19*$Q$19+$Q$20</f>
+        <v>28513.069714187302</v>
+      </c>
+      <c r="B19" s="1">
         <f t="shared" si="1"/>
-        <v>12465.398207303595</v>
-      </c>
-      <c r="L7">
-        <f>_xlfn.STDEV.P(C18:C21)</f>
-        <v>8454.5904287906887</v>
-      </c>
-      <c r="M7">
+        <v>-23634.842546413231</v>
+      </c>
+      <c r="C19" s="3">
         <f t="shared" si="2"/>
-        <v>2077.5663678839323</v>
-      </c>
-      <c r="N7">
-        <f>(K8-K7)/K7</f>
-        <v>1.256583759126618</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="2">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>887.84347826086798</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" t="s">
+        <v>558605782.19374502</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4878.22716777407</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>Just Fine by Standard of Excellence</v>
-      </c>
-      <c r="J8">
+      <c r="K19" t="str">
+        <f t="shared" si="3"/>
+        <v>Promenade by Delmas</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q19" s="8">
+        <f>SLOPE(F2:F33, E2:E33)</f>
+        <v>8095.879305839193</v>
+      </c>
+      <c r="R19" s="9">
+        <f>SLOPE(O2:O11,N2:N11)</f>
+        <v>7630.2125796162045</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20">
+        <f>E20*$Q$19+$Q$20</f>
+        <v>28513.069714187302</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>-1759.7469434065024</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="2"/>
+        <v>3096709.3048285278</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1">
+        <v>26753.3227707808</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="3"/>
+        <v>Scherzo by Koepke</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q20" s="8">
+        <f>INTERCEPT(F2:F33,E2:E33)</f>
+        <v>-20062.206120847855</v>
+      </c>
+      <c r="R20" s="9">
+        <f>INTERCEPT(O2:O11,N2:N11)</f>
+        <v>-17910.187183390361</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21">
+        <f>E21*$Q$19+$Q$20</f>
+        <v>28513.069714187302</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>-18459.859677646502</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="2"/>
+        <v>340766419.31839919</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>10053.210036540801</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="3"/>
+        <v>Nocturne by Bassi</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>0.35876999999999998</v>
+      </c>
+      <c r="R21" s="9">
+        <v>0.79025999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22">
+        <f>E22*$Q$19+$Q$20</f>
+        <v>36608.949020026499</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
+        <v>-21485.7491545468</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="2"/>
+        <v>461637416.73210853</v>
+      </c>
+      <c r="D22" s="2">
         <v>7</v>
       </c>
-      <c r="K8">
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
+        <v>15123.199865479701</v>
+      </c>
+      <c r="G22" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="3"/>
+        <v>Sonata 2nd Movement by Hindemith</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q22" s="11">
+        <f>AVERAGE(C2:C33)</f>
+        <v>995616123.9525491</v>
+      </c>
+      <c r="R22" s="12">
+        <f>AVERAGE(U2:U11)</f>
+        <v>127481601.8636858</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23">
+        <f>E23*$Q$19+$Q$20</f>
+        <v>36608.949020026499</v>
+      </c>
+      <c r="B23" s="1">
         <f t="shared" si="1"/>
-        <v>28129.215145647351</v>
-      </c>
-      <c r="L8">
-        <f>_xlfn.STDEV.P(C22:C23)</f>
-        <v>13006.015280167654</v>
-      </c>
-      <c r="M8">
+        <v>4526.2814057885043</v>
+      </c>
+      <c r="C23" s="3">
         <f t="shared" si="2"/>
-        <v>4018.4593065210502</v>
-      </c>
-      <c r="N8">
-        <f>(K9-K8)/K8</f>
-        <v>0.59410767858254276</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="2"/>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
+        <v>20487223.36438676</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1">
+        <v>41135.230425815003</v>
+      </c>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="3"/>
+        <v>Scene and Air by Bergsen</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24">
+        <f>E24*$Q$19+$Q$20</f>
+        <v>44704.828325865688</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="1"/>
+        <v>-30632.138665527491</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="2"/>
+        <v>938327919.22410429</v>
+      </c>
+      <c r="D24" s="2">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1">
+        <v>14072.689660338199</v>
+      </c>
+      <c r="G24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="3"/>
+        <v>Canzonetta by Pierné</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25">
+        <f>E25*$Q$19+$Q$20</f>
+        <v>44704.828325865688</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="1"/>
+        <v>64705.316707872305</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="2"/>
+        <v>4186778010.2660589</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1">
+        <v>109410.14503373799</v>
+      </c>
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="3"/>
+        <v>Concerto Opus 36 1st Movement by Krommer</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26">
+        <f>E26*$Q$19+$Q$20</f>
+        <v>44704.828325865688</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="1"/>
+        <v>-33664.669451411486</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="2"/>
+        <v>1133309969.2727978</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1">
+        <v>11040.1588744542</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="3"/>
+        <v>Sonata 1st Movement by Saint-Saens</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27">
+        <f>E27*$Q$19+$Q$20</f>
+        <v>52800.707631704878</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="1"/>
+        <v>-38549.975261015279</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="2"/>
+        <v>1486100592.6248901</v>
+      </c>
+      <c r="D27" s="2">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1">
+        <v>14250.7323706896</v>
+      </c>
+      <c r="G27" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="3"/>
+        <v>Sonata 3rd and 4th Movements by Hindemith</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28">
+        <f>E28*$Q$19+$Q$20</f>
+        <v>52800.707631704878</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="1"/>
+        <v>-1194.3332803228768</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="2"/>
+        <v>1426431.9844868034</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28">
+        <v>9</v>
+      </c>
+      <c r="F28" s="1">
+        <v>51606.374351382001</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="3"/>
+        <v>Sonata Movements 2, 3, and 4 by Saint-Saens</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29">
+        <f>E29*$Q$19+$Q$20</f>
+        <v>52800.707631704878</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="1"/>
+        <v>-6721.4569292605811</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="2"/>
+        <v>45177983.251905084</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29">
+        <v>9</v>
+      </c>
+      <c r="F29" s="1">
+        <v>46079.250702444297</v>
+      </c>
+      <c r="G29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="3"/>
+        <v>Solo de Concours by Rabaud</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30">
+        <f>E30*$Q$19+$Q$20</f>
+        <v>60896.586937544067</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="1"/>
+        <v>-1681.3251081803683</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="2"/>
+        <v>2826854.1193977268</v>
+      </c>
+      <c r="D30" s="2">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>59215.261829363699</v>
+      </c>
+      <c r="G30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="3"/>
+        <v>Concerto no. 3 1st and 2nd Movements by Crussell</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31">
+        <f>E31*$Q$19+$Q$20</f>
+        <v>60896.586937544067</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="1"/>
+        <v>141318.2612560339</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="2"/>
+        <v>19970850964.428654</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1">
+        <v>202214.84819357799</v>
+      </c>
+      <c r="G31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="3"/>
+        <v>Concerto no. 3 2nd and 3rd Movements by Crussell</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32">
+        <f>E32*$Q$19+$Q$20</f>
+        <v>60896.586937544067</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="1"/>
+        <v>-24820.195912399067</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="2"/>
+        <v>616042125.12987137</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1">
+        <v>36076.391025145</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="3"/>
+        <v>Solo de Concours by Messager</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33">
+        <f>E33*$Q$19+$Q$20</f>
+        <v>60896.586937544067</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="1"/>
+        <v>-23295.198509171569</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="2"/>
+        <v>542666273.58170927</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>37601.388428372498</v>
+      </c>
+      <c r="G33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="3"/>
+        <v>Sonata no. 2 1st Movement by Stanford</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F35" s="1">
+        <f>MIN(F$2:F$33)</f>
         <v>514.19178082191695</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>Variations on a Theme by Mozart</v>
-      </c>
-      <c r="J9">
-        <v>8</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>44840.9978561768</v>
-      </c>
-      <c r="L9">
-        <f>_xlfn.STDEV.P(C24:C26)</f>
-        <v>45674.063655208105</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="2"/>
-        <v>5605.1247320221</v>
-      </c>
-      <c r="N9">
-        <f>(K10-K9)/K9</f>
-        <v>-0.16790167647070775</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2"/>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1020.793125</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>Loch Lomond by Standard of Excellence</v>
-      </c>
-      <c r="J10">
-        <v>9</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>37312.119141505304</v>
-      </c>
-      <c r="L10">
-        <f>_xlfn.STDEV.P(C27:C29)</f>
-        <v>16462.238482914483</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="2"/>
-        <v>4145.7910157228116</v>
-      </c>
-      <c r="N10">
-        <f>(K11-K10)/K10</f>
-        <v>1.245301909853811</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="2"/>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>2326.8744186046501</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>Theme from Symphony 9 by Beethoven</v>
-      </c>
-      <c r="J11">
-        <v>10</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>83776.972369114796</v>
-      </c>
-      <c r="L11">
-        <f>_xlfn.STDEV.P(C13:C15)</f>
-        <v>9197.6216453278303</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>8377.6972369114792</v>
-      </c>
-      <c r="N11">
-        <f>(K12-K11)/K11</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="2">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>9464.1992307691999</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>Minuet in G by Beethoven</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="2"/>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1">
-        <v>16344.719981735099</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>Gavotte by Gossec</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="2"/>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1">
-        <v>15339.2669023255</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>Song without Words by Tschaikowsky</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>35333.655653513</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>Humoresque by Dvorak</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2"/>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16" s="1">
-        <v>5688.3940240963902</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>The Dancing Doll by Poldini</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="2"/>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1">
-        <v>11433.8131455399</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>Hymn to the Sun by Korsakoff</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>8176.8328541187102</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>Serenade by Drdla</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2"/>
-      <c r="B19">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4878.22716777407</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>Promenade by Delmas</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2"/>
-      <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1">
-        <v>26753.3227707808</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>Scherzo by Koepke</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="2"/>
-      <c r="B21">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
-        <v>10053.210036540801</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>Nocturne by Bassi</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1">
-        <v>15123.199865479701</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonata 2nd Movement by Hindemith</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2"/>
-      <c r="B23">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1">
-        <v>41135.230425815003</v>
-      </c>
-      <c r="D23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v>Scene and Air by Bergsen</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="2">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>8</v>
-      </c>
-      <c r="C24" s="1">
-        <v>14072.689660338199</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v>Canzonetta by Pierné</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2"/>
-      <c r="B25">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="G35" t="str">
+        <f>INDEX(G$2:G$33,MATCH(F35,F$2:F$33))</f>
+        <v>Variations on a Theme</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="E36" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="1">
+        <f>MAX(F$2:F$33)</f>
+        <v>202214.84819357799</v>
+      </c>
+      <c r="G36" t="str">
+        <f>INDEX(G$2:G$33,MATCH(F36,F$2:F$33))</f>
+        <v>Concerto no. 3 2nd and 3rd Movements</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="E37" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="1">
+        <f>LARGE(F2:F33,2)</f>
         <v>109410.14503373799</v>
       </c>
-      <c r="D25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v>Concerto Opus 36 1st Movement by Krommer</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="2"/>
-      <c r="B26">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1">
-        <v>11040.1588744542</v>
-      </c>
-      <c r="D26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" t="s">
-        <v>88</v>
-      </c>
-      <c r="F26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonata 1st Movement by Saint-Saens</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="2">
-        <v>9</v>
-      </c>
-      <c r="B27">
-        <v>9</v>
-      </c>
-      <c r="C27" s="1">
-        <v>14250.7323706896</v>
-      </c>
-      <c r="D27" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonata 3rd and 4th Movements by Hindemith</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="2"/>
-      <c r="B28">
-        <v>9</v>
-      </c>
-      <c r="C28" s="1">
-        <v>51606.374351382001</v>
-      </c>
-      <c r="D28" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonata Movements 2, 3, and 4 by Saint-Saens</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="2"/>
-      <c r="B29">
-        <v>9</v>
-      </c>
-      <c r="C29" s="1">
-        <v>46079.250702444297</v>
-      </c>
-      <c r="D29" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" t="s">
-        <v>54</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v>Solo de Concours by Rabaud</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="2">
-        <v>10</v>
-      </c>
-      <c r="B30">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1">
-        <v>59215.261829363699</v>
-      </c>
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v>Concerto no. 3 1st and 2nd Movements by Crussell</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="2"/>
-      <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="C31" s="1">
-        <v>202214.84819357799</v>
-      </c>
-      <c r="D31" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" t="s">
-        <v>54</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>Concerto no. 3 2nd and 3rd Movements by Crussell</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="2"/>
-      <c r="B32">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1">
-        <v>36076.391025145</v>
-      </c>
-      <c r="D32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" t="s">
-        <v>50</v>
-      </c>
-      <c r="F32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v>Solo de Concours by Messager</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="2"/>
-      <c r="B33">
-        <v>10</v>
-      </c>
-      <c r="C33" s="1">
-        <v>37601.388428372498</v>
-      </c>
-      <c r="D33" t="s">
-        <v>52</v>
-      </c>
-      <c r="E33" t="s">
-        <v>87</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
-        <v>54</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>Sonata no. 2 1st Movement by Stanford</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="B35" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="1">
-        <f>MIN(C$2:C$33)</f>
-        <v>514.19178082191695</v>
-      </c>
-      <c r="D35" t="str">
-        <f>INDEX(D$2:D$33,MATCH(C35,C$2:C$33))</f>
-        <v>Variations on a Theme</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="1">
-        <f>MAX(C$2:C$33)</f>
-        <v>202214.84819357799</v>
-      </c>
-      <c r="D36" t="str">
-        <f>INDEX(D$2:D$33,MATCH(C36,C$2:C$33))</f>
-        <v>Concerto no. 3 2nd and 3rd Movements</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="B37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" s="1">
-        <f>LARGE(C2:C33,2)</f>
-        <v>109410.14503373799</v>
-      </c>
-      <c r="D37" t="str">
-        <f>INDEX(D$2:D$33,MATCH(C37,C$2:C$33))</f>
+      <c r="G37" t="str">
+        <f>INDEX(G$2:G$33,MATCH(F37,F$2:F$33))</f>
         <v>Concerto Opus 36 1st Movement</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="C38" s="1">
-        <f>SMALL(C2:C33,2)</f>
+    <row r="38" spans="1:11">
+      <c r="F38" s="1">
+        <f>SMALL(F2:F33,2)</f>
         <v>535.21621621621603</v>
       </c>
-      <c r="D38" t="s">
+      <c r="G38" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D18:D21"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>